<commit_message>
Se actualiza puntos empalmador
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2025.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2025.xlsx
@@ -190,7 +190,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +205,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="2" builtinId="26"/>
@@ -587,7 +588,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,8 +614,9 @@
       <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7">
-        <v>23.85</v>
+      <c r="C2" s="8">
+        <f>23.85+19.24</f>
+        <v>43.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualiza puntos celadores
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2025.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2025.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,7 +519,8 @@
         <v>18</v>
       </c>
       <c r="C2" s="2">
-        <v>104.49</v>
+        <f>104.49+34.92</f>
+        <v>139.41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -530,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>34.92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -541,7 +542,8 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>104.49</v>
+        <f>104.49+34.92</f>
+        <v>139.41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -587,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Se actualiza excel empalmador
</commit_message>
<xml_diff>
--- a/points-managment/src/assets/PuntosTrabajadores2025.xlsx
+++ b/points-managment/src/assets/PuntosTrabajadores2025.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mes actual cel" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,8 +617,8 @@
         <v>20</v>
       </c>
       <c r="C2" s="8">
-        <f>23.85+19.24</f>
-        <v>43.09</v>
+        <f>23.85+19.24+22.46</f>
+        <v>65.550000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>